<commit_message>
Retirada a Descrição das necessidades
Retirada a Descrição das necessidades
</commit_message>
<xml_diff>
--- a/PDTIC-2018-2020/referencias/objetivos estrategicos.xlsx
+++ b/PDTIC-2018-2020/referencias/objetivos estrategicos.xlsx
@@ -9,10 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9435" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Plan2" sheetId="2" r:id="rId1"/>
+    <sheet name="METAS" sheetId="4" r:id="rId2"/>
+    <sheet name="Plan1" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="60">
   <si>
     <t>Objetivo Estratégico</t>
   </si>
@@ -187,14 +189,70 @@
     <t>2018: 10%
 2019: 40%
 2020: 50%</t>
+  </si>
+  <si>
+    <t>M2018</t>
+  </si>
+  <si>
+    <t>M2019</t>
+  </si>
+  <si>
+    <t>M2020</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>90%</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>8</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>10%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -222,11 +280,39 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -510,15 +596,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
-    <col min="3" max="3" width="29.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="33.42578125" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="25.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -694,4 +780,321 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="34.7109375" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="7.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="3">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="3">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="3">
+        <v>6</v>
+      </c>
+      <c r="E5" s="3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0.93</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="3">
+        <v>4</v>
+      </c>
+      <c r="E7" s="3">
+        <v>4.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="3">
+        <v>60</v>
+      </c>
+      <c r="E9" s="3">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="3">
+        <v>4</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="3">
+        <v>14</v>
+      </c>
+      <c r="E11" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
+      <c r="B12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="3">
+        <v>10</v>
+      </c>
+      <c r="E12" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="11"/>
+      <c r="B13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="3">
+        <v>10</v>
+      </c>
+      <c r="E13" s="3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+      <c r="A14" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="3">
+        <v>2</v>
+      </c>
+      <c r="E14" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="3">
+        <v>30</v>
+      </c>
+      <c r="E15" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D16" s="3">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="11"/>
+      <c r="B17" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D17" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="A16:A17"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>